<commit_message>
Remaking Info Packages with Amy's Guidance
</commit_message>
<xml_diff>
--- a/Solution Documents/BISolutionWorksheets.xlsx
+++ b/Solution Documents/BISolutionWorksheets.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stef.tuder\OneDrive - University of Denver\2_WAREHOUSING\RedwoodSolution\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micha\OneDrive - University of Denver\INFO 4240\RedwoodDW1\RedwoodDW1\Solution Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="30" windowWidth="22980" windowHeight="12165" tabRatio="950" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="36" windowWidth="22980" windowHeight="12168" tabRatio="629" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Team Members" sheetId="7" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="171">
   <si>
     <t>Object Name</t>
   </si>
@@ -291,12 +291,6 @@
     <t>money</t>
   </si>
   <si>
-    <t>nvarchar(50)</t>
-  </si>
-  <si>
-    <t>Dimension  Column</t>
-  </si>
-  <si>
     <t>Generated</t>
   </si>
   <si>
@@ -387,259 +381,163 @@
     <t>Redwood OLTP</t>
   </si>
   <si>
-    <t>RedwoodDW1.dbo.FactContacts</t>
-  </si>
-  <si>
-    <t>Redwood.dbo.publishers</t>
-  </si>
-  <si>
     <t>Redwood.dbo.CustAgentList</t>
   </si>
   <si>
-    <t>Redwood.dbo.Agent</t>
-  </si>
-  <si>
-    <t>RedwoodDW1.dbo.FactContacts.ContactDateKey</t>
-  </si>
-  <si>
-    <t>RedwoodDW1.dbo.FactContacts.AgentKey</t>
-  </si>
-  <si>
-    <t>RedwoodDW1.dbo.FactContacts.PropertyLocationKey</t>
-  </si>
-  <si>
-    <t>Redwood.dbo.CustAgentList.ContactDate</t>
-  </si>
-  <si>
-    <t>Redwood.dbo.Agent.AgentID</t>
-  </si>
-  <si>
     <t>Redwood.dbo.Property.PropertyID</t>
   </si>
   <si>
-    <t>RedwoodDW1.dbo.FactContacts.PropertyTraitsKey</t>
-  </si>
-  <si>
-    <t>RedwoodDW1.dbo.FactContacts.PropertyListing</t>
-  </si>
-  <si>
     <t>Redwood.dbo.Listing</t>
   </si>
   <si>
-    <t>RedwoodDW1.dbo.FactContacts.BidPrice</t>
-  </si>
-  <si>
     <t>Redwood.dbo.CustAgentList.BidPrice</t>
   </si>
   <si>
-    <t>Redwood.dbo.CustAgentList.CommisionRate</t>
-  </si>
-  <si>
-    <t>RedwoodDW1.dbo.FactContacts.Commision</t>
-  </si>
-  <si>
-    <t>numeric(4,4)</t>
-  </si>
-  <si>
-    <t>RedwoodDW1.dbo.DimAgent</t>
-  </si>
-  <si>
-    <t>RedwoodDW1.dbo.DimAgent.Title</t>
-  </si>
-  <si>
     <t>nvarchar(20)</t>
   </si>
   <si>
-    <t>RedwoodDW1.dbo.DimAgent.AgentID</t>
-  </si>
-  <si>
-    <t>RedwoodDW1.dbo.DimAgent.LicenseStatus</t>
-  </si>
-  <si>
-    <t>Redwood.dbo.Agent.Title</t>
-  </si>
-  <si>
-    <t>Redwood.dbo.LicenseStatus.StatusText</t>
-  </si>
-  <si>
-    <t>nvarchar(25)</t>
-  </si>
-  <si>
-    <t>RedwoodDW1.dbo.DimAgent.HireDate</t>
-  </si>
-  <si>
-    <t>Redwood.dbo.Agent.HireDate</t>
-  </si>
-  <si>
-    <t>RedwoodDW1.dbo.DimAgent.LastName</t>
-  </si>
-  <si>
-    <t>RedwoodDW1.dbo.DimAgent.FirstName</t>
-  </si>
-  <si>
-    <t>Redwood.dbo.Agent.FirstName</t>
-  </si>
-  <si>
-    <t>Redwood.dbo.Agent.LastName</t>
-  </si>
-  <si>
     <t>nvarchar(30)</t>
   </si>
   <si>
-    <t>RedwoodDW1.dbo.DimPropertyLocation</t>
-  </si>
-  <si>
     <t>Redwood.dbo.Property</t>
   </si>
   <si>
-    <t>RedwoodDW1.dbo.DimPropertyLocation.PropertyLocationID</t>
-  </si>
-  <si>
-    <t>RedwoodDW1.dbo.DimPropertyLocation.City</t>
-  </si>
-  <si>
     <t>Redwood.dbo.Property.City</t>
   </si>
   <si>
-    <t>RedwoodDW1.dbo.DimPropertyLocation.ZipCode</t>
-  </si>
-  <si>
     <t>Redwood.dbo.Property.ZipCode</t>
   </si>
   <si>
-    <t>RedwoodDW1.dbo.DimPropertyLocation.Address</t>
-  </si>
-  <si>
     <t>Redwood.dbo.Property.Address</t>
   </si>
   <si>
-    <t>RedwoodDW1.dbo.DimPropertyTraits</t>
-  </si>
-  <si>
-    <t>RedwoodDW1.dbo.DimPropertyLocationKey</t>
-  </si>
-  <si>
-    <t>RedwoodDW1.dbo.DimAgentKey</t>
-  </si>
-  <si>
-    <t>RedwoodDW1.dbo.DimPropertyTraitsKey</t>
-  </si>
-  <si>
-    <t>RedwoodDW1.dbo.DimPropertyTraits.PropertyTraitsID</t>
-  </si>
-  <si>
-    <t>RedwoodDW1.dbo.DimPropertyTraits.SalesStatus</t>
-  </si>
-  <si>
     <t>Redwood.dbo.SaleStatus.SaleStatus</t>
   </si>
   <si>
     <t>nvarchar(10)</t>
   </si>
   <si>
-    <t>RedwoodDW1.dbo.DimPropertyTraits.LotSize</t>
-  </si>
-  <si>
     <t>Redwood.dbo.Property.LotSize</t>
   </si>
   <si>
     <t>numeric(4,2)</t>
   </si>
   <si>
-    <t>RedwoodDW1.dbo.DimPropertyTraits.SqFt</t>
-  </si>
-  <si>
     <t>Redwood.dbo.Property.SqFt</t>
   </si>
   <si>
-    <t>RedwoodDW1.dbo.DimPropertyTraits.Bedrooms</t>
-  </si>
-  <si>
     <t>Redwood.dbo.Property.Bedrooms</t>
   </si>
   <si>
-    <t>RedwoodDW1.dbo.DimPropertyTraits.Bathrooms</t>
-  </si>
-  <si>
     <t>Redwood.dbo.Property.Bathrooms</t>
   </si>
   <si>
-    <t>RedwoodDW1.dbo.DimPropertyTraits.Stories</t>
-  </si>
-  <si>
     <t>Redwood.dbo.Property.Stories</t>
   </si>
   <si>
-    <t>RedwoodDW1.dbo.DimPropertyTraits.YearBuilt</t>
-  </si>
-  <si>
     <t>Redwood.dbo.Property.YearBuilt</t>
   </si>
   <si>
     <t>numeric(4,0)</t>
   </si>
   <si>
-    <t>RedwoodDW1.dbo.DimPropertyTraits.AskingPrice</t>
-  </si>
-  <si>
     <t>Redwood.dbo.Property.AskingPrice</t>
   </si>
   <si>
-    <t>RedwoodDW1.dbo.DimPropertyTraits.DaysOnMarket</t>
-  </si>
-  <si>
-    <t>RedwoodDW1.dbo.DimCustomer</t>
-  </si>
-  <si>
-    <t>Redwood.dbo.Customer</t>
-  </si>
-  <si>
-    <t>RedwoodDW1.dbo.DimCustomerKey</t>
-  </si>
-  <si>
-    <t>RedwoodDW1.dbo.DimCustomer.CustomerID</t>
-  </si>
-  <si>
-    <t>Redwood.dbo.Customer.CustomerID</t>
-  </si>
-  <si>
-    <t>RedwoodDW1.dbo.DimCustomer.ContactReason</t>
-  </si>
-  <si>
-    <t>Redwood.dbo.ContactReason.Description</t>
-  </si>
-  <si>
-    <t>RedwoodDW1.dbo.DimCustomer.City</t>
-  </si>
-  <si>
-    <t>Redwood.dbo.Customer.City</t>
-  </si>
-  <si>
-    <t>RedwoodDW1.dbo.DimCustomer.ZipCode</t>
-  </si>
-  <si>
-    <t>Redwood.dbo.Customer.ZipCode</t>
-  </si>
-  <si>
-    <t>RedwoodDW1.dbo.DimCustomer.LastName</t>
-  </si>
-  <si>
-    <t>Redwood.dbo.Customer.LastName</t>
-  </si>
-  <si>
-    <t>RedwoodDW1.dbo.DimCustomer.FirstName</t>
-  </si>
-  <si>
-    <t>Redwood.dbo.Customer.FirstName</t>
-  </si>
-  <si>
-    <t>nvarchar(15)</t>
-  </si>
-  <si>
-    <t>RedwoodDW1.dbo.DimCustomer.PhoneNumber</t>
-  </si>
-  <si>
-    <t>nvarchar(14)</t>
+    <t>RedwoodDW1.dbo.DimProperty</t>
+  </si>
+  <si>
+    <t>RedwoodDW1.dbo.DimProperty.City</t>
+  </si>
+  <si>
+    <t>RedwoodDW1.dbo.DimProperty.ZipCode</t>
+  </si>
+  <si>
+    <t>RedwoodDW1.dbo.DimProperty.Address</t>
+  </si>
+  <si>
+    <t>RedwoodDW1.dbo.DimProperty.LotSize</t>
+  </si>
+  <si>
+    <t>RedwoodDW1.dbo.DimProperty.SqFt</t>
+  </si>
+  <si>
+    <t>RedwoodDW1.dbo.DimProperty.Bedrooms</t>
+  </si>
+  <si>
+    <t>RedwoodDW1.dbo.DimProperty.Bathrooms</t>
+  </si>
+  <si>
+    <t>RedwoodDW1.dbo.DimProperty.Stories</t>
+  </si>
+  <si>
+    <t>RedwoodDW1.dbo.DimProperty.YearBuilt</t>
+  </si>
+  <si>
+    <t>RedwoodDW1.dbo.DimProperty.AskingPrice</t>
+  </si>
+  <si>
+    <t>RedwoodDW1.dbo.DimListing</t>
+  </si>
+  <si>
+    <t>Redwood.dbo.Listing.ListingID</t>
+  </si>
+  <si>
+    <t>Redwood.dbo.Listing.BeginListDate</t>
+  </si>
+  <si>
+    <t>Redwood.dbo.Listing.EndListDate</t>
+  </si>
+  <si>
+    <t>RedwoodDW1.dbo.DimListing.BeginListDate</t>
+  </si>
+  <si>
+    <t>RedwoodDW1.dbo.DimListing.EndListDate</t>
+  </si>
+  <si>
+    <t>RedwoodDW1.dbo.DimListing.DaysonMarket</t>
+  </si>
+  <si>
+    <t>RedwoodDW1.dbo.FactListing</t>
+  </si>
+  <si>
+    <t>Fact Key Column</t>
+  </si>
+  <si>
+    <t>RedwoodDW1.dbo.FactListing.ListFactID</t>
+  </si>
+  <si>
+    <t>RedwoodDW1.dbo.FactListing.SaleStatus</t>
+  </si>
+  <si>
+    <t>RedwoodDW1.dbo.FactListing.Property_SK</t>
+  </si>
+  <si>
+    <t>RedwoodDW1.dbo.DimProperty_SK</t>
+  </si>
+  <si>
+    <t>RedwoodDW1.dbo.DimProperty.PropertyID_AK</t>
+  </si>
+  <si>
+    <t>RedwoodDW1.dbo.FactListing.Listing_SK</t>
+  </si>
+  <si>
+    <t>RedwoodDW1.dbo.DimListing_SK</t>
+  </si>
+  <si>
+    <t>RedwoodDW1.dbo.DimListing.ListingID_AK</t>
+  </si>
+  <si>
+    <t>RedwoodDW1.dbo.FactListing.DaysOnMarket</t>
+  </si>
+  <si>
+    <t>RedwoodDW1.dbo.FactListing.AskingPrice</t>
+  </si>
+  <si>
+    <t>RedwoodDW1.dbo.FactListing.BidPrice</t>
+  </si>
+  <si>
+    <t>Redwood.dbo.CustAgentList.AskingPrice</t>
   </si>
 </sst>
 </file>
@@ -1317,10 +1215,10 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1328,31 +1226,31 @@
         <v>85</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="11" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="12" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="13" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -1362,23 +1260,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:E49"/>
+  <dimension ref="A3:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="60.140625" customWidth="1"/>
-    <col min="2" max="2" width="27.7109375" customWidth="1"/>
+    <col min="1" max="1" width="60.109375" customWidth="1"/>
+    <col min="2" max="2" width="27.6640625" customWidth="1"/>
     <col min="3" max="3" width="45" customWidth="1"/>
-    <col min="4" max="5" width="27.7109375" customWidth="1"/>
+    <col min="4" max="5" width="27.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:5" ht="18.75">
+    <row r="3" spans="1:5" ht="18">
       <c r="A3" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1400,13 +1298,13 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="36" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B5" s="36" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="36" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D5" s="36" t="s">
         <v>8</v>
@@ -1417,13 +1315,13 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="37" t="s">
-        <v>120</v>
+        <v>157</v>
       </c>
       <c r="B6" s="37" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="37" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="D6" s="37" t="s">
         <v>7</v>
@@ -1433,133 +1331,133 @@
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="38" t="s">
-        <v>124</v>
-      </c>
-      <c r="B7" s="38" t="s">
+      <c r="A7" s="36" t="s">
+        <v>159</v>
+      </c>
+      <c r="B7" s="36" t="s">
+        <v>158</v>
+      </c>
+      <c r="C7" s="36" t="s">
+        <v>88</v>
+      </c>
+      <c r="D7" s="36" t="s">
+        <v>89</v>
+      </c>
+      <c r="E7" s="36" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="36" t="s">
+        <v>161</v>
+      </c>
+      <c r="B8" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="38" t="s">
-        <v>127</v>
-      </c>
-      <c r="D7" s="38" t="s">
-        <v>83</v>
-      </c>
-      <c r="E7" s="38" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="38" t="s">
-        <v>125</v>
-      </c>
-      <c r="B8" s="38" t="s">
+      <c r="C8" s="36" t="s">
+        <v>139</v>
+      </c>
+      <c r="D8" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="36" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="36" t="s">
+        <v>164</v>
+      </c>
+      <c r="B9" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="38" t="s">
+      <c r="C9" s="36" t="s">
+        <v>150</v>
+      </c>
+      <c r="D9" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="36" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="36" t="s">
+        <v>160</v>
+      </c>
+      <c r="B10" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="36" t="s">
         <v>128</v>
       </c>
-      <c r="D8" s="38" t="s">
+      <c r="D10" s="36" t="s">
+        <v>129</v>
+      </c>
+      <c r="E10" s="36" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="36" t="s">
+        <v>167</v>
+      </c>
+      <c r="B11" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="36" t="s">
+        <v>88</v>
+      </c>
+      <c r="D11" s="36" t="s">
+        <v>89</v>
+      </c>
+      <c r="E11" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="38" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="38" t="s">
-        <v>126</v>
-      </c>
-      <c r="B9" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="38" t="s">
-        <v>129</v>
-      </c>
-      <c r="D9" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="38" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="38" t="s">
-        <v>130</v>
-      </c>
-      <c r="B10" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="38" t="s">
-        <v>129</v>
-      </c>
-      <c r="D10" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="38" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="38" t="s">
-        <v>133</v>
-      </c>
-      <c r="B11" s="38" t="s">
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="36" t="s">
+        <v>168</v>
+      </c>
+      <c r="B12" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="38" t="s">
-        <v>134</v>
-      </c>
-      <c r="D11" s="38" t="s">
+      <c r="C12" s="36" t="s">
+        <v>170</v>
+      </c>
+      <c r="D12" s="36" t="s">
         <v>87</v>
       </c>
-      <c r="E11" s="38" t="s">
+      <c r="E12" s="36" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="38" t="s">
-        <v>136</v>
-      </c>
-      <c r="B12" s="38" t="s">
+    <row r="13" spans="1:5">
+      <c r="A13" s="36" t="s">
+        <v>169</v>
+      </c>
+      <c r="B13" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="38" t="s">
-        <v>135</v>
-      </c>
-      <c r="D12" s="38" t="s">
-        <v>137</v>
-      </c>
-      <c r="E12" s="38" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="14.45" customHeight="1">
-      <c r="A13" s="38" t="s">
-        <v>131</v>
-      </c>
-      <c r="B13" s="38" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="38" t="s">
-        <v>132</v>
-      </c>
-      <c r="D13" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="E13" s="38" t="s">
-        <v>10</v>
+      <c r="C13" s="36" t="s">
+        <v>121</v>
+      </c>
+      <c r="D13" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="E13" s="36" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="37" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B14" s="37" t="s">
         <v>84</v>
       </c>
       <c r="C14" s="37" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D14" s="37" t="s">
         <v>7</v>
@@ -1570,16 +1468,16 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="38" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B15" s="38" t="s">
         <v>11</v>
       </c>
       <c r="C15" s="38" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D15" s="38" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E15" s="38" t="s">
         <v>10</v>
@@ -1587,13 +1485,13 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="38" t="s">
-        <v>141</v>
+        <v>163</v>
       </c>
       <c r="B16" s="38" t="s">
-        <v>11</v>
+        <v>86</v>
       </c>
       <c r="C16" s="38" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="D16" s="38" t="s">
         <v>10</v>
@@ -1604,118 +1502,118 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="38" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B17" s="38" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C17" s="38" t="s">
-        <v>143</v>
+        <v>125</v>
       </c>
       <c r="D17" s="38" t="s">
-        <v>140</v>
+        <v>123</v>
       </c>
       <c r="E17" s="38" t="s">
-        <v>140</v>
+        <v>123</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="38" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B18" s="38" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C18" s="38" t="s">
-        <v>144</v>
+        <v>126</v>
       </c>
       <c r="D18" s="38" t="s">
-        <v>145</v>
+        <v>122</v>
       </c>
       <c r="E18" s="38" t="s">
-        <v>145</v>
+        <v>122</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="38" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B19" s="38" t="s">
         <v>86</v>
       </c>
       <c r="C19" s="38" t="s">
-        <v>147</v>
+        <v>127</v>
       </c>
       <c r="D19" s="38" t="s">
-        <v>83</v>
+        <v>123</v>
       </c>
       <c r="E19" s="38" t="s">
-        <v>83</v>
+        <v>123</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="38" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="B20" s="38" t="s">
         <v>86</v>
       </c>
       <c r="C20" s="38" t="s">
-        <v>151</v>
+        <v>130</v>
       </c>
       <c r="D20" s="38" t="s">
-        <v>152</v>
+        <v>131</v>
       </c>
       <c r="E20" s="38" t="s">
-        <v>152</v>
+        <v>131</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="38" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="B21" s="38" t="s">
         <v>86</v>
       </c>
       <c r="C21" s="38" t="s">
-        <v>150</v>
+        <v>132</v>
       </c>
       <c r="D21" s="38" t="s">
-        <v>152</v>
+        <v>10</v>
       </c>
       <c r="E21" s="38" t="s">
-        <v>152</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="37" t="s">
-        <v>153</v>
-      </c>
-      <c r="B22" s="37" t="s">
-        <v>84</v>
-      </c>
-      <c r="C22" s="37" t="s">
-        <v>154</v>
-      </c>
-      <c r="D22" s="37" t="s">
-        <v>7</v>
-      </c>
-      <c r="E22" s="37" t="s">
-        <v>7</v>
+      <c r="A22" s="38" t="s">
+        <v>145</v>
+      </c>
+      <c r="B22" s="38" t="s">
+        <v>86</v>
+      </c>
+      <c r="C22" s="38" t="s">
+        <v>133</v>
+      </c>
+      <c r="D22" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" s="38" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="38" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
       <c r="B23" s="38" t="s">
-        <v>11</v>
+        <v>86</v>
       </c>
       <c r="C23" s="38" t="s">
-        <v>90</v>
+        <v>134</v>
       </c>
       <c r="D23" s="38" t="s">
-        <v>91</v>
+        <v>10</v>
       </c>
       <c r="E23" s="38" t="s">
         <v>10</v>
@@ -1723,13 +1621,13 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="38" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="B24" s="38" t="s">
-        <v>11</v>
+        <v>86</v>
       </c>
       <c r="C24" s="38" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="D24" s="38" t="s">
         <v>10</v>
@@ -1740,84 +1638,84 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="38" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="B25" s="38" t="s">
         <v>86</v>
       </c>
       <c r="C25" s="38" t="s">
-        <v>157</v>
+        <v>136</v>
       </c>
       <c r="D25" s="38" t="s">
-        <v>152</v>
+        <v>137</v>
       </c>
       <c r="E25" s="38" t="s">
-        <v>152</v>
+        <v>137</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="38" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="B26" s="38" t="s">
         <v>86</v>
       </c>
       <c r="C26" s="38" t="s">
-        <v>159</v>
+        <v>138</v>
       </c>
       <c r="D26" s="38" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="E26" s="38" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
     </row>
     <row r="27" spans="1:5">
-      <c r="A27" s="38" t="s">
-        <v>160</v>
-      </c>
-      <c r="B27" s="38" t="s">
-        <v>86</v>
-      </c>
-      <c r="C27" s="38" t="s">
-        <v>161</v>
-      </c>
-      <c r="D27" s="38" t="s">
-        <v>152</v>
-      </c>
-      <c r="E27" s="38" t="s">
-        <v>152</v>
+      <c r="A27" s="37" t="s">
+        <v>150</v>
+      </c>
+      <c r="B27" s="37" t="s">
+        <v>84</v>
+      </c>
+      <c r="C27" s="37" t="s">
+        <v>120</v>
+      </c>
+      <c r="D27" s="37" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" s="37" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="37" t="s">
-        <v>162</v>
-      </c>
-      <c r="B28" s="37" t="s">
-        <v>84</v>
-      </c>
-      <c r="C28" s="37" t="s">
-        <v>121</v>
-      </c>
-      <c r="D28" s="37" t="s">
-        <v>7</v>
-      </c>
-      <c r="E28" s="37" t="s">
-        <v>7</v>
+      <c r="A28" s="38" t="s">
+        <v>165</v>
+      </c>
+      <c r="B28" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" s="38" t="s">
+        <v>88</v>
+      </c>
+      <c r="D28" s="38" t="s">
+        <v>89</v>
+      </c>
+      <c r="E28" s="38" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="38" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B29" s="38" t="s">
-        <v>11</v>
+        <v>86</v>
       </c>
       <c r="C29" s="38" t="s">
-        <v>90</v>
+        <v>151</v>
       </c>
       <c r="D29" s="38" t="s">
-        <v>91</v>
+        <v>10</v>
       </c>
       <c r="E29" s="38" t="s">
         <v>10</v>
@@ -1825,341 +1723,69 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="38" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="B30" s="38" t="s">
-        <v>11</v>
+        <v>86</v>
       </c>
       <c r="C30" s="38" t="s">
-        <v>129</v>
+        <v>152</v>
       </c>
       <c r="D30" s="38" t="s">
-        <v>10</v>
+        <v>83</v>
       </c>
       <c r="E30" s="38" t="s">
-        <v>10</v>
+        <v>83</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="38" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="B31" s="38" t="s">
         <v>86</v>
       </c>
       <c r="C31" s="38" t="s">
-        <v>168</v>
+        <v>153</v>
       </c>
       <c r="D31" s="38" t="s">
-        <v>169</v>
+        <v>83</v>
       </c>
       <c r="E31" s="38" t="s">
-        <v>169</v>
+        <v>83</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="38" t="s">
-        <v>170</v>
+        <v>156</v>
       </c>
       <c r="B32" s="38" t="s">
         <v>86</v>
       </c>
       <c r="C32" s="38" t="s">
-        <v>171</v>
+        <v>88</v>
       </c>
       <c r="D32" s="38" t="s">
-        <v>172</v>
+        <v>89</v>
       </c>
       <c r="E32" s="38" t="s">
-        <v>172</v>
+        <v>10</v>
       </c>
     </row>
     <row r="33" spans="1:5">
-      <c r="A33" s="38" t="s">
-        <v>173</v>
-      </c>
-      <c r="B33" s="38" t="s">
-        <v>86</v>
-      </c>
-      <c r="C33" s="38" t="s">
-        <v>174</v>
-      </c>
-      <c r="D33" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="E33" s="38" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
-      <c r="A34" s="38" t="s">
-        <v>175</v>
-      </c>
-      <c r="B34" s="38" t="s">
-        <v>86</v>
-      </c>
-      <c r="C34" s="38" t="s">
-        <v>176</v>
-      </c>
-      <c r="D34" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="E34" s="38" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
-      <c r="A35" s="38" t="s">
-        <v>177</v>
-      </c>
-      <c r="B35" s="38" t="s">
-        <v>86</v>
-      </c>
-      <c r="C35" s="38" t="s">
-        <v>178</v>
-      </c>
-      <c r="D35" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="E35" s="38" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
-      <c r="A36" s="38" t="s">
-        <v>179</v>
-      </c>
-      <c r="B36" s="38" t="s">
-        <v>86</v>
-      </c>
-      <c r="C36" s="38" t="s">
-        <v>180</v>
-      </c>
-      <c r="D36" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="E36" s="38" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
-      <c r="A37" s="38" t="s">
-        <v>181</v>
-      </c>
-      <c r="B37" s="38" t="s">
-        <v>86</v>
-      </c>
-      <c r="C37" s="38" t="s">
-        <v>182</v>
-      </c>
-      <c r="D37" s="38" t="s">
-        <v>183</v>
-      </c>
-      <c r="E37" s="38" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5">
-      <c r="A38" s="38" t="s">
-        <v>184</v>
-      </c>
-      <c r="B38" s="38" t="s">
-        <v>86</v>
-      </c>
-      <c r="C38" s="38" t="s">
-        <v>185</v>
-      </c>
-      <c r="D38" s="38" t="s">
-        <v>172</v>
-      </c>
-      <c r="E38" s="38" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5">
-      <c r="A39" s="38" t="s">
-        <v>186</v>
-      </c>
-      <c r="B39" s="38" t="s">
-        <v>86</v>
-      </c>
-      <c r="C39" s="38" t="s">
-        <v>90</v>
-      </c>
-      <c r="D39" s="38" t="s">
-        <v>91</v>
-      </c>
-      <c r="E39" s="38" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5">
-      <c r="A40" s="37" t="s">
-        <v>187</v>
-      </c>
-      <c r="B40" s="37" t="s">
-        <v>84</v>
-      </c>
-      <c r="C40" s="37" t="s">
-        <v>188</v>
-      </c>
-      <c r="D40" s="37" t="s">
-        <v>7</v>
-      </c>
-      <c r="E40" s="37" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5">
-      <c r="A41" s="38" t="s">
-        <v>189</v>
-      </c>
-      <c r="B41" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="C41" s="38" t="s">
-        <v>90</v>
-      </c>
-      <c r="D41" s="38" t="s">
-        <v>91</v>
-      </c>
-      <c r="E41" s="38" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5">
-      <c r="A42" s="38" t="s">
-        <v>190</v>
-      </c>
-      <c r="B42" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="C42" s="38" t="s">
-        <v>191</v>
-      </c>
-      <c r="D42" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="E42" s="38" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5">
-      <c r="A43" s="38" t="s">
-        <v>192</v>
-      </c>
-      <c r="B43" s="38" t="s">
-        <v>86</v>
-      </c>
-      <c r="C43" s="38" t="s">
-        <v>193</v>
-      </c>
-      <c r="D43" s="38" t="s">
-        <v>88</v>
-      </c>
-      <c r="E43" s="38" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5">
-      <c r="A44" s="38" t="s">
-        <v>194</v>
-      </c>
-      <c r="B44" s="38" t="s">
-        <v>86</v>
-      </c>
-      <c r="C44" s="38" t="s">
-        <v>195</v>
-      </c>
-      <c r="D44" s="38" t="s">
-        <v>140</v>
-      </c>
-      <c r="E44" s="38" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5">
-      <c r="A45" s="38" t="s">
-        <v>196</v>
-      </c>
-      <c r="B45" s="38" t="s">
-        <v>86</v>
-      </c>
-      <c r="C45" s="38" t="s">
-        <v>197</v>
-      </c>
-      <c r="D45" s="38" t="s">
-        <v>169</v>
-      </c>
-      <c r="E45" s="38" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5">
-      <c r="A46" s="38" t="s">
-        <v>198</v>
-      </c>
-      <c r="B46" s="38" t="s">
-        <v>86</v>
-      </c>
-      <c r="C46" s="38" t="s">
-        <v>199</v>
-      </c>
-      <c r="D46" s="38" t="s">
-        <v>140</v>
-      </c>
-      <c r="E46" s="38" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5">
-      <c r="A47" s="38" t="s">
-        <v>200</v>
-      </c>
-      <c r="B47" s="38" t="s">
-        <v>86</v>
-      </c>
-      <c r="C47" s="38" t="s">
-        <v>201</v>
-      </c>
-      <c r="D47" s="38" t="s">
-        <v>202</v>
-      </c>
-      <c r="E47" s="38" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5">
-      <c r="A48" s="38" t="s">
-        <v>203</v>
-      </c>
-      <c r="B48" s="38" t="s">
-        <v>86</v>
-      </c>
-      <c r="C48" s="38" t="s">
-        <v>90</v>
-      </c>
-      <c r="D48" s="38" t="s">
-        <v>91</v>
-      </c>
-      <c r="E48" s="38" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5">
-      <c r="A49" s="35" t="s">
+      <c r="A33" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B49" s="35" t="s">
+      <c r="B33" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="C49" s="35" t="s">
+      <c r="C33" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="D49" s="35" t="s">
+      <c r="D33" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="E49" s="35" t="s">
+      <c r="E33" s="35" t="s">
         <v>9</v>
       </c>
     </row>
@@ -2177,10 +1803,10 @@
       <selection activeCell="L2" sqref="A2:L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:12">
@@ -2188,37 +1814,37 @@
         <v>12</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C2" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="E2" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="F2" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="G2" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="F2" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="G2" s="14" t="s">
-        <v>97</v>
-      </c>
       <c r="H2" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="I2" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="J2" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="I2" s="14" t="s">
+      <c r="K2" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="J2" s="14" t="s">
+      <c r="L2" s="14" t="s">
         <v>95</v>
-      </c>
-      <c r="K2" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="L2" s="14" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -2229,7 +1855,7 @@
         <v>28</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D3" s="16"/>
       <c r="E3" s="16"/>
@@ -2241,7 +1867,7 @@
       <c r="K3" s="11"/>
       <c r="L3" s="11"/>
     </row>
-    <row r="4" spans="1:12" ht="15.75" thickBot="1">
+    <row r="4" spans="1:12" ht="15" thickBot="1">
       <c r="A4" s="3" t="s">
         <v>28</v>
       </c>
@@ -2252,7 +1878,7 @@
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
       <c r="F4" s="17" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G4" s="16"/>
       <c r="H4" s="16"/>
@@ -2274,7 +1900,7 @@
       <c r="F5" s="22"/>
       <c r="G5" s="22"/>
       <c r="H5" s="23" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="I5" s="22"/>
       <c r="J5" s="22"/>
@@ -2294,7 +1920,7 @@
       <c r="F6" s="26"/>
       <c r="G6" s="26"/>
       <c r="H6" s="27" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="I6" s="28"/>
       <c r="J6" s="26"/>
@@ -2314,14 +1940,14 @@
       <c r="F7" s="26"/>
       <c r="G7" s="26"/>
       <c r="H7" s="27" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I7" s="26"/>
       <c r="J7" s="26"/>
       <c r="K7" s="26"/>
       <c r="L7" s="29"/>
     </row>
-    <row r="8" spans="1:12" ht="15.75" thickBot="1">
+    <row r="8" spans="1:12" ht="15" thickBot="1">
       <c r="A8" s="30" t="s">
         <v>32</v>
       </c>
@@ -2334,7 +1960,7 @@
       <c r="F8" s="31"/>
       <c r="G8" s="31"/>
       <c r="H8" s="32" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I8" s="31"/>
       <c r="J8" s="31"/>
@@ -2354,16 +1980,16 @@
       <c r="F9" s="11"/>
       <c r="G9" s="11"/>
       <c r="H9" s="18" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="I9" s="17" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="J9" s="16"/>
       <c r="K9" s="16"/>
       <c r="L9" s="11"/>
     </row>
-    <row r="10" spans="1:12" ht="30">
+    <row r="10" spans="1:12" ht="28.8">
       <c r="A10" s="15" t="s">
         <v>34</v>
       </c>
@@ -2379,7 +2005,7 @@
       <c r="I10" s="13"/>
       <c r="J10" s="13"/>
       <c r="K10" s="20" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="L10" s="19"/>
     </row>
@@ -2406,13 +2032,13 @@
       <selection activeCell="E2" sqref="A2:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="35.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.5703125" customWidth="1"/>
-    <col min="3" max="3" width="53.140625" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.5546875" customWidth="1"/>
+    <col min="3" max="3" width="53.109375" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:5">
@@ -2982,18 +2608,18 @@
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="48.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.85546875" customWidth="1"/>
-    <col min="3" max="3" width="63.42578125" customWidth="1"/>
-    <col min="4" max="4" width="19.5703125" customWidth="1"/>
-    <col min="5" max="5" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="48.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.88671875" customWidth="1"/>
+    <col min="3" max="3" width="63.44140625" customWidth="1"/>
+    <col min="4" max="4" width="19.5546875" customWidth="1"/>
+    <col min="5" max="5" width="23.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" ht="18">
+    <row r="2" spans="1:5" ht="17.399999999999999">
       <c r="A2" s="40" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B2" s="40"/>
       <c r="C2" s="39"/>
@@ -3005,7 +2631,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="41" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C3" s="41" t="s">
         <v>2</v>
@@ -3014,7 +2640,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="41" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -3108,15 +2734,15 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="40.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" ht="18.75">
+    <row r="2" spans="1:2" ht="18">
       <c r="A2" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -3138,7 +2764,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Adding a new visio diagram to the solution documents and cleaned up our current solutions folder
</commit_message>
<xml_diff>
--- a/Solution Documents/BISolutionWorksheets.xlsx
+++ b/Solution Documents/BISolutionWorksheets.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="168">
   <si>
     <t>Object Name</t>
   </si>
@@ -441,9 +441,6 @@
     <t>numeric(4,0)</t>
   </si>
   <si>
-    <t>Redwood.dbo.Property.AskingPrice</t>
-  </si>
-  <si>
     <t>RedwoodDW1.dbo.DimProperty</t>
   </si>
   <si>
@@ -474,9 +471,6 @@
     <t>RedwoodDW1.dbo.DimProperty.YearBuilt</t>
   </si>
   <si>
-    <t>RedwoodDW1.dbo.DimProperty.AskingPrice</t>
-  </si>
-  <si>
     <t>RedwoodDW1.dbo.DimListing</t>
   </si>
   <si>
@@ -495,36 +489,24 @@
     <t>RedwoodDW1.dbo.DimListing.EndListDate</t>
   </si>
   <si>
-    <t>RedwoodDW1.dbo.DimListing.DaysonMarket</t>
-  </si>
-  <si>
     <t>RedwoodDW1.dbo.FactListing</t>
   </si>
   <si>
     <t>Fact Key Column</t>
   </si>
   <si>
-    <t>RedwoodDW1.dbo.FactListing.ListFactID</t>
-  </si>
-  <si>
     <t>RedwoodDW1.dbo.FactListing.SaleStatus</t>
   </si>
   <si>
     <t>RedwoodDW1.dbo.FactListing.Property_SK</t>
   </si>
   <si>
-    <t>RedwoodDW1.dbo.DimProperty_SK</t>
-  </si>
-  <si>
     <t>RedwoodDW1.dbo.DimProperty.PropertyID_AK</t>
   </si>
   <si>
     <t>RedwoodDW1.dbo.FactListing.Listing_SK</t>
   </si>
   <si>
-    <t>RedwoodDW1.dbo.DimListing_SK</t>
-  </si>
-  <si>
     <t>RedwoodDW1.dbo.DimListing.ListingID_AK</t>
   </si>
   <si>
@@ -538,6 +520,15 @@
   </si>
   <si>
     <t>Redwood.dbo.CustAgentList.AskingPrice</t>
+  </si>
+  <si>
+    <t>RedwoodDW1.dbo.FactListing.ListFact_SK</t>
+  </si>
+  <si>
+    <t>RedwoodDW1.dbo.DimProperty.Property_SK</t>
+  </si>
+  <si>
+    <t>RedwoodDW1.dbo.DimListing.Listing_SK</t>
   </si>
 </sst>
 </file>
@@ -1260,10 +1251,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:E33"/>
+  <dimension ref="A3:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1315,7 +1306,7 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="37" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B6" s="37" t="s">
         <v>3</v>
@@ -1332,10 +1323,10 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="36" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="B7" s="36" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C7" s="36" t="s">
         <v>88</v>
@@ -1349,13 +1340,13 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="36" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B8" s="36" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="36" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D8" s="36" t="s">
         <v>10</v>
@@ -1366,13 +1357,13 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="36" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="B9" s="36" t="s">
         <v>11</v>
       </c>
       <c r="C9" s="36" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D9" s="36" t="s">
         <v>10</v>
@@ -1383,7 +1374,7 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="36" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B10" s="36" t="s">
         <v>6</v>
@@ -1400,7 +1391,7 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="36" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="B11" s="36" t="s">
         <v>6</v>
@@ -1417,13 +1408,13 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="36" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="B12" s="36" t="s">
         <v>6</v>
       </c>
       <c r="C12" s="36" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="D12" s="36" t="s">
         <v>87</v>
@@ -1434,7 +1425,7 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="36" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="B13" s="36" t="s">
         <v>6</v>
@@ -1451,7 +1442,7 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="37" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B14" s="37" t="s">
         <v>84</v>
@@ -1468,7 +1459,7 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="38" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="B15" s="38" t="s">
         <v>11</v>
@@ -1485,7 +1476,7 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="38" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="B16" s="38" t="s">
         <v>86</v>
@@ -1502,7 +1493,7 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="38" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B17" s="38" t="s">
         <v>86</v>
@@ -1519,7 +1510,7 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="38" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B18" s="38" t="s">
         <v>86</v>
@@ -1536,7 +1527,7 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="38" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B19" s="38" t="s">
         <v>86</v>
@@ -1553,7 +1544,7 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="38" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B20" s="38" t="s">
         <v>86</v>
@@ -1570,7 +1561,7 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="38" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B21" s="38" t="s">
         <v>86</v>
@@ -1587,7 +1578,7 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="38" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B22" s="38" t="s">
         <v>86</v>
@@ -1604,7 +1595,7 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="38" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B23" s="38" t="s">
         <v>86</v>
@@ -1621,7 +1612,7 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="38" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B24" s="38" t="s">
         <v>86</v>
@@ -1638,7 +1629,7 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="38" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B25" s="38" t="s">
         <v>86</v>
@@ -1654,51 +1645,51 @@
       </c>
     </row>
     <row r="26" spans="1:5">
-      <c r="A26" s="38" t="s">
-        <v>149</v>
-      </c>
-      <c r="B26" s="38" t="s">
-        <v>86</v>
-      </c>
-      <c r="C26" s="38" t="s">
-        <v>138</v>
-      </c>
-      <c r="D26" s="38" t="s">
-        <v>131</v>
-      </c>
-      <c r="E26" s="38" t="s">
-        <v>131</v>
+      <c r="A26" s="37" t="s">
+        <v>148</v>
+      </c>
+      <c r="B26" s="37" t="s">
+        <v>84</v>
+      </c>
+      <c r="C26" s="37" t="s">
+        <v>120</v>
+      </c>
+      <c r="D26" s="37" t="s">
+        <v>7</v>
+      </c>
+      <c r="E26" s="37" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:5">
-      <c r="A27" s="37" t="s">
-        <v>150</v>
-      </c>
-      <c r="B27" s="37" t="s">
-        <v>84</v>
-      </c>
-      <c r="C27" s="37" t="s">
-        <v>120</v>
-      </c>
-      <c r="D27" s="37" t="s">
-        <v>7</v>
-      </c>
-      <c r="E27" s="37" t="s">
-        <v>7</v>
+      <c r="A27" s="38" t="s">
+        <v>167</v>
+      </c>
+      <c r="B27" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" s="38" t="s">
+        <v>88</v>
+      </c>
+      <c r="D27" s="38" t="s">
+        <v>89</v>
+      </c>
+      <c r="E27" s="38" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="38" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="B28" s="38" t="s">
-        <v>11</v>
+        <v>86</v>
       </c>
       <c r="C28" s="38" t="s">
-        <v>88</v>
+        <v>149</v>
       </c>
       <c r="D28" s="38" t="s">
-        <v>89</v>
+        <v>10</v>
       </c>
       <c r="E28" s="38" t="s">
         <v>10</v>
@@ -1706,30 +1697,30 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="38" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="B29" s="38" t="s">
         <v>86</v>
       </c>
       <c r="C29" s="38" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D29" s="38" t="s">
-        <v>10</v>
+        <v>83</v>
       </c>
       <c r="E29" s="38" t="s">
-        <v>10</v>
+        <v>83</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="38" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B30" s="38" t="s">
         <v>86</v>
       </c>
       <c r="C30" s="38" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D30" s="38" t="s">
         <v>83</v>
@@ -1739,53 +1730,19 @@
       </c>
     </row>
     <row r="31" spans="1:5">
-      <c r="A31" s="38" t="s">
-        <v>155</v>
-      </c>
-      <c r="B31" s="38" t="s">
-        <v>86</v>
-      </c>
-      <c r="C31" s="38" t="s">
-        <v>153</v>
-      </c>
-      <c r="D31" s="38" t="s">
-        <v>83</v>
-      </c>
-      <c r="E31" s="38" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="A32" s="38" t="s">
-        <v>156</v>
-      </c>
-      <c r="B32" s="38" t="s">
-        <v>86</v>
-      </c>
-      <c r="C32" s="38" t="s">
-        <v>88</v>
-      </c>
-      <c r="D32" s="38" t="s">
-        <v>89</v>
-      </c>
-      <c r="E32" s="38" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
-      <c r="A33" s="35" t="s">
+      <c r="A31" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B33" s="35" t="s">
+      <c r="B31" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="C33" s="35" t="s">
+      <c r="C31" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="D33" s="35" t="s">
+      <c r="D31" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="E33" s="35" t="s">
+      <c r="E31" s="35" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated solution documents with discussed changes and altered fact table to be FactDaysOnMarket
</commit_message>
<xml_diff>
--- a/Solution Documents/BISolutionWorksheets.xlsx
+++ b/Solution Documents/BISolutionWorksheets.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micha\OneDrive - University of Denver\INFO 4240\RedwoodDW1\RedwoodDW1\Solution Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stef.tuder\OneDrive - University of Denver\2_WAREHOUSING\RedwoodSolution\Solution Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="36" windowWidth="22980" windowHeight="12168" tabRatio="629" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="30" windowWidth="22980" windowHeight="12165" tabRatio="629" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Team Members" sheetId="7" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="180">
   <si>
     <t>Object Name</t>
   </si>
@@ -489,24 +489,12 @@
     <t>RedwoodDW1.dbo.DimListing.EndListDate</t>
   </si>
   <si>
-    <t>RedwoodDW1.dbo.FactListing</t>
-  </si>
-  <si>
-    <t>Fact Key Column</t>
-  </si>
-  <si>
-    <t>RedwoodDW1.dbo.FactListing.SaleStatus</t>
-  </si>
-  <si>
     <t>RedwoodDW1.dbo.FactListing.Property_SK</t>
   </si>
   <si>
     <t>RedwoodDW1.dbo.DimProperty.PropertyID_AK</t>
   </si>
   <si>
-    <t>RedwoodDW1.dbo.FactListing.Listing_SK</t>
-  </si>
-  <si>
     <t>RedwoodDW1.dbo.DimListing.ListingID_AK</t>
   </si>
   <si>
@@ -522,13 +510,61 @@
     <t>Redwood.dbo.CustAgentList.AskingPrice</t>
   </si>
   <si>
-    <t>RedwoodDW1.dbo.FactListing.ListFact_SK</t>
-  </si>
-  <si>
     <t>RedwoodDW1.dbo.DimProperty.Property_SK</t>
   </si>
   <si>
     <t>RedwoodDW1.dbo.DimListing.Listing_SK</t>
+  </si>
+  <si>
+    <t>RedwoodDW1.dbo.FactDaysOnMarket</t>
+  </si>
+  <si>
+    <t>RedwoodDW1.dbo.DimProperty.SaleStatus</t>
+  </si>
+  <si>
+    <t>RedwoodDW1.dbo.DimAgentKey</t>
+  </si>
+  <si>
+    <t>RedwoodDW1.dbo.DimAgent.AgentID</t>
+  </si>
+  <si>
+    <t>Redwood.dbo.Agent.AgentID</t>
+  </si>
+  <si>
+    <t>RedwoodDW1.dbo.DimAgent.Title</t>
+  </si>
+  <si>
+    <t>Dimension  Column</t>
+  </si>
+  <si>
+    <t>Redwood.dbo.Agent.Title</t>
+  </si>
+  <si>
+    <t>RedwoodDW1.dbo.DimAgent</t>
+  </si>
+  <si>
+    <t>Redwood.dbo.Agent</t>
+  </si>
+  <si>
+    <t>RedwoodDW1.dbo.DimAgent.HireDate</t>
+  </si>
+  <si>
+    <t>Redwood.dbo.Agent.HireDate</t>
+  </si>
+  <si>
+    <t>RedwoodDW1.dbo.DimAgent.Gender</t>
+  </si>
+  <si>
+    <t>Redwood.dbo.Agent.Gender</t>
+  </si>
+  <si>
+    <t>RedwoodDW1.dbo.DimAgent.Age</t>
+  </si>
+  <si>
+    <t>nchar(1)</t>
+  </si>
+  <si>
+    <t>RedwoodDW1.dbo.FactListing.Agent_SK</t>
   </si>
 </sst>
 </file>
@@ -1206,10 +1242,10 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1251,21 +1287,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:E31"/>
+  <dimension ref="A3:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="60.109375" customWidth="1"/>
-    <col min="2" max="2" width="27.6640625" customWidth="1"/>
+    <col min="1" max="1" width="60.140625" customWidth="1"/>
+    <col min="2" max="2" width="27.7109375" customWidth="1"/>
     <col min="3" max="3" width="45" customWidth="1"/>
-    <col min="4" max="5" width="27.6640625" customWidth="1"/>
+    <col min="4" max="5" width="27.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:5" ht="18">
+    <row r="3" spans="1:5" ht="18.75">
       <c r="A3" s="1" t="s">
         <v>90</v>
       </c>
@@ -1306,7 +1342,7 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="37" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="B6" s="37" t="s">
         <v>3</v>
@@ -1323,16 +1359,16 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="36" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="B7" s="36" t="s">
-        <v>155</v>
+        <v>11</v>
       </c>
       <c r="C7" s="36" t="s">
-        <v>88</v>
+        <v>138</v>
       </c>
       <c r="D7" s="36" t="s">
-        <v>89</v>
+        <v>10</v>
       </c>
       <c r="E7" s="36" t="s">
         <v>10</v>
@@ -1340,13 +1376,13 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="36" t="s">
-        <v>157</v>
+        <v>179</v>
       </c>
       <c r="B8" s="36" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="36" t="s">
-        <v>138</v>
+        <v>171</v>
       </c>
       <c r="D8" s="36" t="s">
         <v>10</v>
@@ -1357,16 +1393,16 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="36" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B9" s="36" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C9" s="36" t="s">
-        <v>148</v>
+        <v>88</v>
       </c>
       <c r="D9" s="36" t="s">
-        <v>10</v>
+        <v>89</v>
       </c>
       <c r="E9" s="36" t="s">
         <v>10</v>
@@ -1374,200 +1410,200 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="36" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B10" s="36" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="36" t="s">
-        <v>128</v>
+        <v>160</v>
       </c>
       <c r="D10" s="36" t="s">
-        <v>129</v>
+        <v>87</v>
       </c>
       <c r="E10" s="36" t="s">
-        <v>129</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="36" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B11" s="36" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="36" t="s">
+        <v>121</v>
+      </c>
+      <c r="D11" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="E11" s="36" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="37" t="s">
+        <v>138</v>
+      </c>
+      <c r="B12" s="37" t="s">
+        <v>84</v>
+      </c>
+      <c r="C12" s="37" t="s">
+        <v>124</v>
+      </c>
+      <c r="D12" s="37" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="37" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="38" t="s">
+        <v>161</v>
+      </c>
+      <c r="B13" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="38" t="s">
         <v>88</v>
       </c>
-      <c r="D11" s="36" t="s">
+      <c r="D13" s="38" t="s">
         <v>89</v>
       </c>
-      <c r="E11" s="36" t="s">
+      <c r="E13" s="38" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="36" t="s">
-        <v>162</v>
-      </c>
-      <c r="B12" s="36" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="36" t="s">
+    <row r="14" spans="1:5">
+      <c r="A14" s="38" t="s">
+        <v>155</v>
+      </c>
+      <c r="B14" s="38" t="s">
+        <v>86</v>
+      </c>
+      <c r="C14" s="38" t="s">
+        <v>119</v>
+      </c>
+      <c r="D14" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="38" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="36" t="s">
         <v>164</v>
       </c>
-      <c r="D12" s="36" t="s">
-        <v>87</v>
-      </c>
-      <c r="E12" s="36" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="36" t="s">
-        <v>163</v>
-      </c>
-      <c r="B13" s="36" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="36" t="s">
-        <v>121</v>
-      </c>
-      <c r="D13" s="36" t="s">
-        <v>87</v>
-      </c>
-      <c r="E13" s="36" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="37" t="s">
-        <v>138</v>
-      </c>
-      <c r="B14" s="37" t="s">
-        <v>84</v>
-      </c>
-      <c r="C14" s="37" t="s">
-        <v>124</v>
-      </c>
-      <c r="D14" s="37" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" s="37" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="38" t="s">
-        <v>166</v>
-      </c>
-      <c r="B15" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="38" t="s">
-        <v>88</v>
-      </c>
-      <c r="D15" s="38" t="s">
-        <v>89</v>
-      </c>
-      <c r="E15" s="38" t="s">
-        <v>10</v>
+      <c r="B15" s="36" t="s">
+        <v>86</v>
+      </c>
+      <c r="C15" s="36" t="s">
+        <v>128</v>
+      </c>
+      <c r="D15" s="36" t="s">
+        <v>129</v>
+      </c>
+      <c r="E15" s="36" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="38" t="s">
-        <v>158</v>
+        <v>139</v>
       </c>
       <c r="B16" s="38" t="s">
         <v>86</v>
       </c>
       <c r="C16" s="38" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="D16" s="38" t="s">
-        <v>10</v>
+        <v>123</v>
       </c>
       <c r="E16" s="38" t="s">
-        <v>10</v>
+        <v>123</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="38" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B17" s="38" t="s">
         <v>86</v>
       </c>
       <c r="C17" s="38" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D17" s="38" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E17" s="38" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="38" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B18" s="38" t="s">
         <v>86</v>
       </c>
       <c r="C18" s="38" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D18" s="38" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E18" s="38" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="38" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B19" s="38" t="s">
         <v>86</v>
       </c>
       <c r="C19" s="38" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="D19" s="38" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="E19" s="38" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="38" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B20" s="38" t="s">
         <v>86</v>
       </c>
       <c r="C20" s="38" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="D20" s="38" t="s">
-        <v>131</v>
+        <v>10</v>
       </c>
       <c r="E20" s="38" t="s">
-        <v>131</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="38" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B21" s="38" t="s">
         <v>86</v>
       </c>
       <c r="C21" s="38" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D21" s="38" t="s">
         <v>10</v>
@@ -1578,13 +1614,13 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="38" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B22" s="38" t="s">
         <v>86</v>
       </c>
       <c r="C22" s="38" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D22" s="38" t="s">
         <v>10</v>
@@ -1595,13 +1631,13 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="38" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B23" s="38" t="s">
         <v>86</v>
       </c>
       <c r="C23" s="38" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D23" s="38" t="s">
         <v>10</v>
@@ -1612,67 +1648,67 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="38" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B24" s="38" t="s">
         <v>86</v>
       </c>
       <c r="C24" s="38" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D24" s="38" t="s">
+        <v>137</v>
+      </c>
+      <c r="E24" s="38" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="37" t="s">
+        <v>148</v>
+      </c>
+      <c r="B25" s="37" t="s">
+        <v>84</v>
+      </c>
+      <c r="C25" s="37" t="s">
+        <v>120</v>
+      </c>
+      <c r="D25" s="37" t="s">
+        <v>7</v>
+      </c>
+      <c r="E25" s="37" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="38" t="s">
+        <v>162</v>
+      </c>
+      <c r="B26" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" s="38" t="s">
+        <v>88</v>
+      </c>
+      <c r="D26" s="38" t="s">
+        <v>89</v>
+      </c>
+      <c r="E26" s="38" t="s">
         <v>10</v>
-      </c>
-      <c r="E24" s="38" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="38" t="s">
-        <v>147</v>
-      </c>
-      <c r="B25" s="38" t="s">
-        <v>86</v>
-      </c>
-      <c r="C25" s="38" t="s">
-        <v>136</v>
-      </c>
-      <c r="D25" s="38" t="s">
-        <v>137</v>
-      </c>
-      <c r="E25" s="38" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="37" t="s">
-        <v>148</v>
-      </c>
-      <c r="B26" s="37" t="s">
-        <v>84</v>
-      </c>
-      <c r="C26" s="37" t="s">
-        <v>120</v>
-      </c>
-      <c r="D26" s="37" t="s">
-        <v>7</v>
-      </c>
-      <c r="E26" s="37" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="38" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="B27" s="38" t="s">
-        <v>11</v>
+        <v>86</v>
       </c>
       <c r="C27" s="38" t="s">
-        <v>88</v>
+        <v>149</v>
       </c>
       <c r="D27" s="38" t="s">
-        <v>89</v>
+        <v>10</v>
       </c>
       <c r="E27" s="38" t="s">
         <v>10</v>
@@ -1680,30 +1716,30 @@
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="38" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="B28" s="38" t="s">
         <v>86</v>
       </c>
       <c r="C28" s="38" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D28" s="38" t="s">
-        <v>10</v>
+        <v>83</v>
       </c>
       <c r="E28" s="38" t="s">
-        <v>10</v>
+        <v>83</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="38" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B29" s="38" t="s">
         <v>86</v>
       </c>
       <c r="C29" s="38" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D29" s="38" t="s">
         <v>83</v>
@@ -1713,36 +1749,138 @@
       </c>
     </row>
     <row r="30" spans="1:5">
-      <c r="A30" s="38" t="s">
-        <v>153</v>
-      </c>
-      <c r="B30" s="38" t="s">
+      <c r="A30" s="37" t="s">
+        <v>171</v>
+      </c>
+      <c r="B30" s="37" t="s">
+        <v>84</v>
+      </c>
+      <c r="C30" s="37" t="s">
+        <v>172</v>
+      </c>
+      <c r="D30" s="37" t="s">
+        <v>7</v>
+      </c>
+      <c r="E30" s="37" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="38" t="s">
+        <v>165</v>
+      </c>
+      <c r="B31" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31" s="38" t="s">
+        <v>88</v>
+      </c>
+      <c r="D31" s="38" t="s">
+        <v>89</v>
+      </c>
+      <c r="E31" s="38" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="38" t="s">
+        <v>166</v>
+      </c>
+      <c r="B32" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32" s="38" t="s">
+        <v>167</v>
+      </c>
+      <c r="D32" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="E32" s="38" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="38" t="s">
+        <v>168</v>
+      </c>
+      <c r="B33" s="38" t="s">
+        <v>169</v>
+      </c>
+      <c r="C33" s="38" t="s">
+        <v>170</v>
+      </c>
+      <c r="D33" s="38" t="s">
+        <v>122</v>
+      </c>
+      <c r="E33" s="38" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="38" t="s">
+        <v>173</v>
+      </c>
+      <c r="B34" s="38" t="s">
         <v>86</v>
       </c>
-      <c r="C30" s="38" t="s">
-        <v>151</v>
-      </c>
-      <c r="D30" s="38" t="s">
+      <c r="C34" s="38" t="s">
+        <v>174</v>
+      </c>
+      <c r="D34" s="38" t="s">
         <v>83</v>
       </c>
-      <c r="E30" s="38" t="s">
+      <c r="E34" s="38" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
-      <c r="A31" s="35" t="s">
+    <row r="35" spans="1:5">
+      <c r="A35" s="38" t="s">
+        <v>175</v>
+      </c>
+      <c r="B35" s="38" t="s">
+        <v>86</v>
+      </c>
+      <c r="C35" s="38" t="s">
+        <v>176</v>
+      </c>
+      <c r="D35" s="38" t="s">
+        <v>178</v>
+      </c>
+      <c r="E35" s="38" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="38" t="s">
+        <v>177</v>
+      </c>
+      <c r="B36" s="38" t="s">
+        <v>86</v>
+      </c>
+      <c r="C36" s="38" t="s">
+        <v>88</v>
+      </c>
+      <c r="D36" s="38" t="s">
+        <v>89</v>
+      </c>
+      <c r="E36" s="38" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B31" s="35" t="s">
+      <c r="B37" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="C31" s="35" t="s">
+      <c r="C37" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="D31" s="35" t="s">
+      <c r="D37" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="E31" s="35" t="s">
+      <c r="E37" s="35" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1760,10 +1898,10 @@
       <selection activeCell="L2" sqref="A2:L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:12">
@@ -1824,7 +1962,7 @@
       <c r="K3" s="11"/>
       <c r="L3" s="11"/>
     </row>
-    <row r="4" spans="1:12" ht="15" thickBot="1">
+    <row r="4" spans="1:12" ht="15.75" thickBot="1">
       <c r="A4" s="3" t="s">
         <v>28</v>
       </c>
@@ -1904,7 +2042,7 @@
       <c r="K7" s="26"/>
       <c r="L7" s="29"/>
     </row>
-    <row r="8" spans="1:12" ht="15" thickBot="1">
+    <row r="8" spans="1:12" ht="15.75" thickBot="1">
       <c r="A8" s="30" t="s">
         <v>32</v>
       </c>
@@ -1946,7 +2084,7 @@
       <c r="K9" s="16"/>
       <c r="L9" s="11"/>
     </row>
-    <row r="10" spans="1:12" ht="28.8">
+    <row r="10" spans="1:12" ht="30">
       <c r="A10" s="15" t="s">
         <v>34</v>
       </c>
@@ -1989,13 +2127,13 @@
       <selection activeCell="E2" sqref="A2:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="35.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.5546875" customWidth="1"/>
-    <col min="3" max="3" width="53.109375" customWidth="1"/>
-    <col min="4" max="4" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.5703125" customWidth="1"/>
+    <col min="3" max="3" width="53.140625" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:5">
@@ -2565,16 +2703,16 @@
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="48.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.88671875" customWidth="1"/>
-    <col min="3" max="3" width="63.44140625" customWidth="1"/>
-    <col min="4" max="4" width="19.5546875" customWidth="1"/>
-    <col min="5" max="5" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="48.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.85546875" customWidth="1"/>
+    <col min="3" max="3" width="63.42578125" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" customWidth="1"/>
+    <col min="5" max="5" width="23.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" ht="17.399999999999999">
+    <row r="2" spans="1:5" ht="18">
       <c r="A2" s="40" t="s">
         <v>105</v>
       </c>
@@ -2691,13 +2829,13 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="40.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" ht="18">
+    <row r="2" spans="1:2" ht="18.75">
       <c r="A2" s="1" t="s">
         <v>106</v>
       </c>
@@ -2721,7 +2859,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fixed Diagram and xls
</commit_message>
<xml_diff>
--- a/Solution Documents/BISolutionWorksheets.xlsx
+++ b/Solution Documents/BISolutionWorksheets.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18229"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stef.tuder\OneDrive - University of Denver\2_WAREHOUSING\RedwoodSolution\Solution Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\migue\Source\Repos\RedwoodDW1\Solution Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="181">
   <si>
     <t>Object Name</t>
   </si>
@@ -471,100 +471,103 @@
     <t>RedwoodDW1.dbo.DimProperty.YearBuilt</t>
   </si>
   <si>
-    <t>RedwoodDW1.dbo.DimListing</t>
-  </si>
-  <si>
-    <t>Redwood.dbo.Listing.ListingID</t>
+    <t>RedwoodDW1.dbo.FactListing.Property_SK</t>
+  </si>
+  <si>
+    <t>RedwoodDW1.dbo.DimProperty.PropertyID_AK</t>
+  </si>
+  <si>
+    <t>RedwoodDW1.dbo.FactListing.AskingPrice</t>
+  </si>
+  <si>
+    <t>RedwoodDW1.dbo.FactListing.BidPrice</t>
+  </si>
+  <si>
+    <t>Redwood.dbo.CustAgentList.AskingPrice</t>
+  </si>
+  <si>
+    <t>RedwoodDW1.dbo.DimProperty.Property_SK</t>
+  </si>
+  <si>
+    <t>RedwoodDW1.dbo.FactDaysOnMarket</t>
+  </si>
+  <si>
+    <t>RedwoodDW1.dbo.DimProperty.SaleStatus</t>
+  </si>
+  <si>
+    <t>RedwoodDW1.dbo.DimAgentKey</t>
+  </si>
+  <si>
+    <t>RedwoodDW1.dbo.DimAgent.AgentID</t>
+  </si>
+  <si>
+    <t>Redwood.dbo.Agent.AgentID</t>
+  </si>
+  <si>
+    <t>RedwoodDW1.dbo.DimAgent.Title</t>
+  </si>
+  <si>
+    <t>Dimension  Column</t>
+  </si>
+  <si>
+    <t>Redwood.dbo.Agent.Title</t>
+  </si>
+  <si>
+    <t>RedwoodDW1.dbo.DimAgent</t>
+  </si>
+  <si>
+    <t>Redwood.dbo.Agent</t>
+  </si>
+  <si>
+    <t>RedwoodDW1.dbo.DimAgent.HireDate</t>
+  </si>
+  <si>
+    <t>Redwood.dbo.Agent.HireDate</t>
+  </si>
+  <si>
+    <t>RedwoodDW1.dbo.DimAgent.Gender</t>
+  </si>
+  <si>
+    <t>Redwood.dbo.Agent.Gender</t>
+  </si>
+  <si>
+    <t>RedwoodDW1.dbo.DimAgent.Age</t>
+  </si>
+  <si>
+    <t>nchar(1)</t>
+  </si>
+  <si>
+    <t>RedwoodDW1.dbo.FactListing.Agent_SK</t>
+  </si>
+  <si>
+    <t>RedwoodDW1.dbo.DimDate</t>
+  </si>
+  <si>
+    <t>RedwoodDW1.dbo.DimDate.Date_SK</t>
+  </si>
+  <si>
+    <t>RedwoodDW1.dbo.DimDate.Date</t>
+  </si>
+  <si>
+    <t>RedwoodDW1.dbo.DimDate.Month</t>
+  </si>
+  <si>
+    <t>RedwoodDW1.dbo.DimDate.Quarter</t>
+  </si>
+  <si>
+    <t>RedwoodDW1.dbo.DimDate.Year</t>
+  </si>
+  <si>
+    <t>RedwoodDW1.dbo.FactListing.ContactDate</t>
+  </si>
+  <si>
+    <t>RedwoodDW1.dbo.FactListing.BeginListDate</t>
+  </si>
+  <si>
+    <t>Redwood.dbo.CustAgentList.ContactDate</t>
   </si>
   <si>
     <t>Redwood.dbo.Listing.BeginListDate</t>
-  </si>
-  <si>
-    <t>Redwood.dbo.Listing.EndListDate</t>
-  </si>
-  <si>
-    <t>RedwoodDW1.dbo.DimListing.BeginListDate</t>
-  </si>
-  <si>
-    <t>RedwoodDW1.dbo.DimListing.EndListDate</t>
-  </si>
-  <si>
-    <t>RedwoodDW1.dbo.FactListing.Property_SK</t>
-  </si>
-  <si>
-    <t>RedwoodDW1.dbo.DimProperty.PropertyID_AK</t>
-  </si>
-  <si>
-    <t>RedwoodDW1.dbo.DimListing.ListingID_AK</t>
-  </si>
-  <si>
-    <t>RedwoodDW1.dbo.FactListing.DaysOnMarket</t>
-  </si>
-  <si>
-    <t>RedwoodDW1.dbo.FactListing.AskingPrice</t>
-  </si>
-  <si>
-    <t>RedwoodDW1.dbo.FactListing.BidPrice</t>
-  </si>
-  <si>
-    <t>Redwood.dbo.CustAgentList.AskingPrice</t>
-  </si>
-  <si>
-    <t>RedwoodDW1.dbo.DimProperty.Property_SK</t>
-  </si>
-  <si>
-    <t>RedwoodDW1.dbo.DimListing.Listing_SK</t>
-  </si>
-  <si>
-    <t>RedwoodDW1.dbo.FactDaysOnMarket</t>
-  </si>
-  <si>
-    <t>RedwoodDW1.dbo.DimProperty.SaleStatus</t>
-  </si>
-  <si>
-    <t>RedwoodDW1.dbo.DimAgentKey</t>
-  </si>
-  <si>
-    <t>RedwoodDW1.dbo.DimAgent.AgentID</t>
-  </si>
-  <si>
-    <t>Redwood.dbo.Agent.AgentID</t>
-  </si>
-  <si>
-    <t>RedwoodDW1.dbo.DimAgent.Title</t>
-  </si>
-  <si>
-    <t>Dimension  Column</t>
-  </si>
-  <si>
-    <t>Redwood.dbo.Agent.Title</t>
-  </si>
-  <si>
-    <t>RedwoodDW1.dbo.DimAgent</t>
-  </si>
-  <si>
-    <t>Redwood.dbo.Agent</t>
-  </si>
-  <si>
-    <t>RedwoodDW1.dbo.DimAgent.HireDate</t>
-  </si>
-  <si>
-    <t>Redwood.dbo.Agent.HireDate</t>
-  </si>
-  <si>
-    <t>RedwoodDW1.dbo.DimAgent.Gender</t>
-  </si>
-  <si>
-    <t>Redwood.dbo.Agent.Gender</t>
-  </si>
-  <si>
-    <t>RedwoodDW1.dbo.DimAgent.Age</t>
-  </si>
-  <si>
-    <t>nchar(1)</t>
-  </si>
-  <si>
-    <t>RedwoodDW1.dbo.FactListing.Agent_SK</t>
   </si>
 </sst>
 </file>
@@ -1242,10 +1245,10 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1287,21 +1290,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:E37"/>
+  <dimension ref="A3:E39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="60.140625" customWidth="1"/>
-    <col min="2" max="2" width="27.7109375" customWidth="1"/>
+    <col min="1" max="1" width="60.1328125" customWidth="1"/>
+    <col min="2" max="2" width="27.73046875" customWidth="1"/>
     <col min="3" max="3" width="45" customWidth="1"/>
-    <col min="4" max="5" width="27.7109375" customWidth="1"/>
+    <col min="4" max="5" width="27.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:5" ht="18.75">
+    <row r="3" spans="1:5" ht="18">
       <c r="A3" s="1" t="s">
         <v>90</v>
       </c>
@@ -1342,7 +1345,7 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="37" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="B6" s="37" t="s">
         <v>3</v>
@@ -1359,7 +1362,7 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="36" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B7" s="36" t="s">
         <v>11</v>
@@ -1376,13 +1379,13 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="36" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="B8" s="36" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="36" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="D8" s="36" t="s">
         <v>10</v>
@@ -1393,47 +1396,47 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="36" t="s">
-        <v>157</v>
+        <v>177</v>
       </c>
       <c r="B9" s="36" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C9" s="36" t="s">
-        <v>88</v>
+        <v>179</v>
       </c>
       <c r="D9" s="36" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="E9" s="36" t="s">
-        <v>10</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="36" t="s">
-        <v>158</v>
+        <v>178</v>
       </c>
       <c r="B10" s="36" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C10" s="36" t="s">
-        <v>160</v>
+        <v>180</v>
       </c>
       <c r="D10" s="36" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E10" s="36" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="36" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="B11" s="36" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C11" s="36" t="s">
-        <v>121</v>
+        <v>152</v>
       </c>
       <c r="D11" s="36" t="s">
         <v>87</v>
@@ -1443,167 +1446,167 @@
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="37" t="s">
+      <c r="A12" s="36" t="s">
+        <v>151</v>
+      </c>
+      <c r="B12" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="36" t="s">
+        <v>121</v>
+      </c>
+      <c r="D12" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="E12" s="36" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="37" t="s">
         <v>138</v>
       </c>
-      <c r="B12" s="37" t="s">
+      <c r="B13" s="37" t="s">
         <v>84</v>
       </c>
-      <c r="C12" s="37" t="s">
+      <c r="C13" s="37" t="s">
         <v>124</v>
       </c>
-      <c r="D12" s="37" t="s">
+      <c r="D13" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="E12" s="37" t="s">
+      <c r="E13" s="37" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="38" t="s">
-        <v>161</v>
-      </c>
-      <c r="B13" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="38" t="s">
-        <v>88</v>
-      </c>
-      <c r="D13" s="38" t="s">
-        <v>89</v>
-      </c>
-      <c r="E13" s="38" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="38" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B14" s="38" t="s">
-        <v>86</v>
+        <v>11</v>
       </c>
       <c r="C14" s="38" t="s">
-        <v>119</v>
+        <v>88</v>
       </c>
       <c r="D14" s="38" t="s">
-        <v>10</v>
+        <v>89</v>
       </c>
       <c r="E14" s="38" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="36" t="s">
-        <v>164</v>
-      </c>
-      <c r="B15" s="36" t="s">
+      <c r="A15" s="38" t="s">
+        <v>149</v>
+      </c>
+      <c r="B15" s="38" t="s">
         <v>86</v>
       </c>
-      <c r="C15" s="36" t="s">
+      <c r="C15" s="38" t="s">
+        <v>119</v>
+      </c>
+      <c r="D15" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="38" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="36" t="s">
+        <v>155</v>
+      </c>
+      <c r="B16" s="36" t="s">
+        <v>86</v>
+      </c>
+      <c r="C16" s="36" t="s">
         <v>128</v>
       </c>
-      <c r="D15" s="36" t="s">
+      <c r="D16" s="36" t="s">
         <v>129</v>
       </c>
-      <c r="E15" s="36" t="s">
+      <c r="E16" s="36" t="s">
         <v>129</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="38" t="s">
-        <v>139</v>
-      </c>
-      <c r="B16" s="38" t="s">
-        <v>86</v>
-      </c>
-      <c r="C16" s="38" t="s">
-        <v>125</v>
-      </c>
-      <c r="D16" s="38" t="s">
-        <v>123</v>
-      </c>
-      <c r="E16" s="38" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="38" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B17" s="38" t="s">
         <v>86</v>
       </c>
       <c r="C17" s="38" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D17" s="38" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E17" s="38" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="38" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B18" s="38" t="s">
         <v>86</v>
       </c>
       <c r="C18" s="38" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D18" s="38" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E18" s="38" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="38" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B19" s="38" t="s">
         <v>86</v>
       </c>
       <c r="C19" s="38" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D19" s="38" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="E19" s="38" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="38" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B20" s="38" t="s">
         <v>86</v>
       </c>
       <c r="C20" s="38" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D20" s="38" t="s">
-        <v>10</v>
+        <v>131</v>
       </c>
       <c r="E20" s="38" t="s">
-        <v>10</v>
+        <v>131</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="38" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B21" s="38" t="s">
         <v>86</v>
       </c>
       <c r="C21" s="38" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D21" s="38" t="s">
         <v>10</v>
@@ -1614,13 +1617,13 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="38" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B22" s="38" t="s">
         <v>86</v>
       </c>
       <c r="C22" s="38" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D22" s="38" t="s">
         <v>10</v>
@@ -1631,13 +1634,13 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="38" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B23" s="38" t="s">
         <v>86</v>
       </c>
       <c r="C23" s="38" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D23" s="38" t="s">
         <v>10</v>
@@ -1648,67 +1651,67 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="38" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B24" s="38" t="s">
         <v>86</v>
       </c>
       <c r="C24" s="38" t="s">
+        <v>135</v>
+      </c>
+      <c r="D24" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" s="38" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="38" t="s">
+        <v>147</v>
+      </c>
+      <c r="B25" s="38" t="s">
+        <v>86</v>
+      </c>
+      <c r="C25" s="38" t="s">
         <v>136</v>
       </c>
-      <c r="D24" s="38" t="s">
+      <c r="D25" s="38" t="s">
         <v>137</v>
       </c>
-      <c r="E24" s="38" t="s">
+      <c r="E25" s="38" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="37" t="s">
-        <v>148</v>
-      </c>
-      <c r="B25" s="37" t="s">
+    <row r="26" spans="1:5">
+      <c r="A26" s="37" t="s">
+        <v>171</v>
+      </c>
+      <c r="B26" s="37" t="s">
         <v>84</v>
       </c>
-      <c r="C25" s="37" t="s">
+      <c r="C26" s="37" t="s">
         <v>120</v>
       </c>
-      <c r="D25" s="37" t="s">
+      <c r="D26" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="E25" s="37" t="s">
+      <c r="E26" s="37" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="38" t="s">
-        <v>162</v>
-      </c>
-      <c r="B26" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="C26" s="38" t="s">
-        <v>88</v>
-      </c>
-      <c r="D26" s="38" t="s">
-        <v>89</v>
-      </c>
-      <c r="E26" s="38" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="38" t="s">
-        <v>156</v>
+        <v>172</v>
       </c>
       <c r="B27" s="38" t="s">
-        <v>86</v>
+        <v>11</v>
       </c>
       <c r="C27" s="38" t="s">
-        <v>149</v>
+        <v>88</v>
       </c>
       <c r="D27" s="38" t="s">
-        <v>10</v>
+        <v>89</v>
       </c>
       <c r="E27" s="38" t="s">
         <v>10</v>
@@ -1716,16 +1719,16 @@
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="38" t="s">
-        <v>152</v>
+        <v>176</v>
       </c>
       <c r="B28" s="38" t="s">
         <v>86</v>
       </c>
       <c r="C28" s="38" t="s">
-        <v>150</v>
+        <v>88</v>
       </c>
       <c r="D28" s="38" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="E28" s="38" t="s">
         <v>83</v>
@@ -1733,44 +1736,44 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="38" t="s">
-        <v>153</v>
+        <v>175</v>
       </c>
       <c r="B29" s="38" t="s">
         <v>86</v>
       </c>
       <c r="C29" s="38" t="s">
-        <v>151</v>
+        <v>88</v>
       </c>
       <c r="D29" s="38" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="E29" s="38" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="30" spans="1:5">
-      <c r="A30" s="37" t="s">
-        <v>171</v>
-      </c>
-      <c r="B30" s="37" t="s">
-        <v>84</v>
-      </c>
-      <c r="C30" s="37" t="s">
-        <v>172</v>
-      </c>
-      <c r="D30" s="37" t="s">
-        <v>7</v>
-      </c>
-      <c r="E30" s="37" t="s">
-        <v>7</v>
+      <c r="A30" s="38" t="s">
+        <v>174</v>
+      </c>
+      <c r="B30" s="38" t="s">
+        <v>86</v>
+      </c>
+      <c r="C30" s="38" t="s">
+        <v>88</v>
+      </c>
+      <c r="D30" s="38" t="s">
+        <v>89</v>
+      </c>
+      <c r="E30" s="38" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="38" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
       <c r="B31" s="38" t="s">
-        <v>11</v>
+        <v>86</v>
       </c>
       <c r="C31" s="38" t="s">
         <v>88</v>
@@ -1779,108 +1782,142 @@
         <v>89</v>
       </c>
       <c r="E31" s="38" t="s">
-        <v>10</v>
+        <v>83</v>
       </c>
     </row>
     <row r="32" spans="1:5">
-      <c r="A32" s="38" t="s">
-        <v>166</v>
-      </c>
-      <c r="B32" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="C32" s="38" t="s">
-        <v>167</v>
-      </c>
-      <c r="D32" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="E32" s="38" t="s">
-        <v>10</v>
+      <c r="A32" s="37" t="s">
+        <v>162</v>
+      </c>
+      <c r="B32" s="37" t="s">
+        <v>84</v>
+      </c>
+      <c r="C32" s="37" t="s">
+        <v>163</v>
+      </c>
+      <c r="D32" s="37" t="s">
+        <v>7</v>
+      </c>
+      <c r="E32" s="37" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="38" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="B33" s="38" t="s">
-        <v>169</v>
+        <v>11</v>
       </c>
       <c r="C33" s="38" t="s">
-        <v>170</v>
+        <v>88</v>
       </c>
       <c r="D33" s="38" t="s">
-        <v>122</v>
+        <v>89</v>
       </c>
       <c r="E33" s="38" t="s">
-        <v>122</v>
+        <v>10</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="38" t="s">
-        <v>173</v>
+        <v>157</v>
       </c>
       <c r="B34" s="38" t="s">
-        <v>86</v>
+        <v>11</v>
       </c>
       <c r="C34" s="38" t="s">
-        <v>174</v>
+        <v>158</v>
       </c>
       <c r="D34" s="38" t="s">
-        <v>83</v>
+        <v>10</v>
       </c>
       <c r="E34" s="38" t="s">
-        <v>83</v>
+        <v>10</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="38" t="s">
-        <v>175</v>
+        <v>159</v>
       </c>
       <c r="B35" s="38" t="s">
-        <v>86</v>
+        <v>160</v>
       </c>
       <c r="C35" s="38" t="s">
-        <v>176</v>
+        <v>161</v>
       </c>
       <c r="D35" s="38" t="s">
-        <v>178</v>
+        <v>122</v>
       </c>
       <c r="E35" s="38" t="s">
-        <v>178</v>
+        <v>122</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="38" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="B36" s="38" t="s">
         <v>86</v>
       </c>
       <c r="C36" s="38" t="s">
+        <v>165</v>
+      </c>
+      <c r="D36" s="38" t="s">
+        <v>83</v>
+      </c>
+      <c r="E36" s="38" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="38" t="s">
+        <v>166</v>
+      </c>
+      <c r="B37" s="38" t="s">
+        <v>86</v>
+      </c>
+      <c r="C37" s="38" t="s">
+        <v>167</v>
+      </c>
+      <c r="D37" s="38" t="s">
+        <v>169</v>
+      </c>
+      <c r="E37" s="38" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="38" t="s">
+        <v>168</v>
+      </c>
+      <c r="B38" s="38" t="s">
+        <v>86</v>
+      </c>
+      <c r="C38" s="38" t="s">
         <v>88</v>
       </c>
-      <c r="D36" s="38" t="s">
+      <c r="D38" s="38" t="s">
         <v>89</v>
       </c>
-      <c r="E36" s="38" t="s">
+      <c r="E38" s="38" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
-      <c r="A37" s="35" t="s">
+    <row r="39" spans="1:5">
+      <c r="A39" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B37" s="35" t="s">
+      <c r="B39" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="C37" s="35" t="s">
+      <c r="C39" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="D37" s="35" t="s">
+      <c r="D39" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="E37" s="35" t="s">
+      <c r="E39" s="35" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1898,10 +1935,10 @@
       <selection activeCell="L2" sqref="A2:L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:12">
@@ -1962,7 +1999,7 @@
       <c r="K3" s="11"/>
       <c r="L3" s="11"/>
     </row>
-    <row r="4" spans="1:12" ht="15.75" thickBot="1">
+    <row r="4" spans="1:12" ht="14.65" thickBot="1">
       <c r="A4" s="3" t="s">
         <v>28</v>
       </c>
@@ -2042,7 +2079,7 @@
       <c r="K7" s="26"/>
       <c r="L7" s="29"/>
     </row>
-    <row r="8" spans="1:12" ht="15.75" thickBot="1">
+    <row r="8" spans="1:12" ht="14.65" thickBot="1">
       <c r="A8" s="30" t="s">
         <v>32</v>
       </c>
@@ -2084,7 +2121,7 @@
       <c r="K9" s="16"/>
       <c r="L9" s="11"/>
     </row>
-    <row r="10" spans="1:12" ht="30">
+    <row r="10" spans="1:12" ht="28.5">
       <c r="A10" s="15" t="s">
         <v>34</v>
       </c>
@@ -2127,13 +2164,13 @@
       <selection activeCell="E2" sqref="A2:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="35.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.5703125" customWidth="1"/>
-    <col min="3" max="3" width="53.140625" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.59765625" customWidth="1"/>
+    <col min="3" max="3" width="53.1328125" customWidth="1"/>
+    <col min="4" max="4" width="20.73046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:5">
@@ -2703,16 +2740,16 @@
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="48.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.85546875" customWidth="1"/>
-    <col min="3" max="3" width="63.42578125" customWidth="1"/>
-    <col min="4" max="4" width="19.5703125" customWidth="1"/>
-    <col min="5" max="5" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="48.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.86328125" customWidth="1"/>
+    <col min="3" max="3" width="63.3984375" customWidth="1"/>
+    <col min="4" max="4" width="19.59765625" customWidth="1"/>
+    <col min="5" max="5" width="23.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" ht="18">
+    <row r="2" spans="1:5" ht="17.649999999999999">
       <c r="A2" s="40" t="s">
         <v>105</v>
       </c>
@@ -2829,13 +2866,13 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="40.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" ht="18.75">
+    <row r="2" spans="1:2" ht="18">
       <c r="A2" s="1" t="s">
         <v>106</v>
       </c>
@@ -2859,7 +2896,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fixes to solution worksheet
</commit_message>
<xml_diff>
--- a/Solution Documents/BISolutionWorksheets.xlsx
+++ b/Solution Documents/BISolutionWorksheets.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\migue\Source\Repos\RedwoodDW1\Solution Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stef.tuder\OneDrive - University of Denver\2_WAREHOUSING\RedwoodSolution\Solution Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -471,21 +471,9 @@
     <t>RedwoodDW1.dbo.DimProperty.YearBuilt</t>
   </si>
   <si>
-    <t>RedwoodDW1.dbo.FactListing.Property_SK</t>
-  </si>
-  <si>
     <t>RedwoodDW1.dbo.DimProperty.PropertyID_AK</t>
   </si>
   <si>
-    <t>RedwoodDW1.dbo.FactListing.AskingPrice</t>
-  </si>
-  <si>
-    <t>RedwoodDW1.dbo.FactListing.BidPrice</t>
-  </si>
-  <si>
-    <t>Redwood.dbo.CustAgentList.AskingPrice</t>
-  </si>
-  <si>
     <t>RedwoodDW1.dbo.DimProperty.Property_SK</t>
   </si>
   <si>
@@ -534,9 +522,6 @@
     <t>nchar(1)</t>
   </si>
   <si>
-    <t>RedwoodDW1.dbo.FactListing.Agent_SK</t>
-  </si>
-  <si>
     <t>RedwoodDW1.dbo.DimDate</t>
   </si>
   <si>
@@ -555,12 +540,6 @@
     <t>RedwoodDW1.dbo.DimDate.Year</t>
   </si>
   <si>
-    <t>RedwoodDW1.dbo.FactListing.ContactDate</t>
-  </si>
-  <si>
-    <t>RedwoodDW1.dbo.FactListing.BeginListDate</t>
-  </si>
-  <si>
     <t>Redwood.dbo.CustAgentList.ContactDate</t>
   </si>
   <si>
@@ -571,6 +550,27 @@
   </si>
   <si>
     <t>Redwood.dbo.Agent.DateOfBirth</t>
+  </si>
+  <si>
+    <t>RedwoodDW1.dbo.FactDaysOnMarket.Property_SK</t>
+  </si>
+  <si>
+    <t>RedwoodDW1.dbo.FactDaysOnMarket.Agent_SK</t>
+  </si>
+  <si>
+    <t>RedwoodDW1.dbo.FactDaysOnMarket.ContactDate</t>
+  </si>
+  <si>
+    <t>RedwoodDW1.dbo.FactDaysOnMarket.BeginListDate</t>
+  </si>
+  <si>
+    <t>RedwoodDW1.dbo.FactDaysOnMarket.AskingPrice</t>
+  </si>
+  <si>
+    <t>RedwoodDW1.dbo.FactDaysOnMarket.BidPrice</t>
+  </si>
+  <si>
+    <t>Redwood.dbo.Listing.AskingPrice</t>
   </si>
 </sst>
 </file>
@@ -1248,10 +1248,10 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15.73046875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1295,19 +1295,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="60.1328125" customWidth="1"/>
-    <col min="2" max="2" width="27.73046875" customWidth="1"/>
+    <col min="1" max="1" width="60.140625" customWidth="1"/>
+    <col min="2" max="2" width="27.7109375" customWidth="1"/>
     <col min="3" max="3" width="45" customWidth="1"/>
-    <col min="4" max="5" width="27.73046875" customWidth="1"/>
+    <col min="4" max="5" width="27.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:5" ht="18">
+    <row r="3" spans="1:5" ht="18.75">
       <c r="A3" s="1" t="s">
         <v>90</v>
       </c>
@@ -1348,7 +1348,7 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="37" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B6" s="37" t="s">
         <v>3</v>
@@ -1365,7 +1365,7 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="36" t="s">
-        <v>148</v>
+        <v>175</v>
       </c>
       <c r="B7" s="36" t="s">
         <v>11</v>
@@ -1382,13 +1382,13 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="36" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="B8" s="36" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="36" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="D8" s="36" t="s">
         <v>10</v>
@@ -1399,13 +1399,13 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="36" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B9" s="36" t="s">
         <v>11</v>
       </c>
       <c r="C9" s="36" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="D9" s="36" t="s">
         <v>83</v>
@@ -1416,13 +1416,13 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="36" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B10" s="36" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="36" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="D10" s="36" t="s">
         <v>83</v>
@@ -1433,13 +1433,13 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="36" t="s">
-        <v>150</v>
+        <v>179</v>
       </c>
       <c r="B11" s="36" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="36" t="s">
-        <v>152</v>
+        <v>181</v>
       </c>
       <c r="D11" s="36" t="s">
         <v>87</v>
@@ -1450,7 +1450,7 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="36" t="s">
-        <v>151</v>
+        <v>180</v>
       </c>
       <c r="B12" s="36" t="s">
         <v>6</v>
@@ -1484,7 +1484,7 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="38" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B14" s="38" t="s">
         <v>11</v>
@@ -1501,7 +1501,7 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="38" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B15" s="38" t="s">
         <v>86</v>
@@ -1518,7 +1518,7 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="36" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B16" s="36" t="s">
         <v>86</v>
@@ -1688,7 +1688,7 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="37" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="B26" s="37" t="s">
         <v>84</v>
@@ -1705,7 +1705,7 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="38" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="B27" s="38" t="s">
         <v>11</v>
@@ -1722,7 +1722,7 @@
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="38" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="B28" s="38" t="s">
         <v>86</v>
@@ -1739,7 +1739,7 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="38" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="B29" s="38" t="s">
         <v>86</v>
@@ -1756,7 +1756,7 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="38" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="B30" s="38" t="s">
         <v>86</v>
@@ -1773,7 +1773,7 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="38" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="B31" s="38" t="s">
         <v>86</v>
@@ -1790,13 +1790,13 @@
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="37" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B32" s="37" t="s">
         <v>84</v>
       </c>
       <c r="C32" s="37" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="D32" s="37" t="s">
         <v>7</v>
@@ -1807,7 +1807,7 @@
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="38" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B33" s="38" t="s">
         <v>11</v>
@@ -1824,13 +1824,13 @@
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="38" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B34" s="38" t="s">
         <v>11</v>
       </c>
       <c r="C34" s="38" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="D34" s="38" t="s">
         <v>10</v>
@@ -1841,13 +1841,13 @@
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="38" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B35" s="38" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C35" s="38" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="D35" s="38" t="s">
         <v>122</v>
@@ -1858,13 +1858,13 @@
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="38" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B36" s="38" t="s">
         <v>86</v>
       </c>
       <c r="C36" s="38" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="D36" s="38" t="s">
         <v>83</v>
@@ -1875,30 +1875,30 @@
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="38" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B37" s="38" t="s">
         <v>86</v>
       </c>
       <c r="C37" s="38" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="D37" s="38" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="E37" s="38" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="38" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="B38" s="38" t="s">
         <v>86</v>
       </c>
       <c r="C38" s="38" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="D38" s="38" t="s">
         <v>83</v>
@@ -1938,10 +1938,10 @@
       <selection activeCell="L2" sqref="A2:L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:12">
@@ -2002,7 +2002,7 @@
       <c r="K3" s="11"/>
       <c r="L3" s="11"/>
     </row>
-    <row r="4" spans="1:12" ht="14.65" thickBot="1">
+    <row r="4" spans="1:12" ht="15.75" thickBot="1">
       <c r="A4" s="3" t="s">
         <v>28</v>
       </c>
@@ -2082,7 +2082,7 @@
       <c r="K7" s="26"/>
       <c r="L7" s="29"/>
     </row>
-    <row r="8" spans="1:12" ht="14.65" thickBot="1">
+    <row r="8" spans="1:12" ht="15.75" thickBot="1">
       <c r="A8" s="30" t="s">
         <v>32</v>
       </c>
@@ -2124,7 +2124,7 @@
       <c r="K9" s="16"/>
       <c r="L9" s="11"/>
     </row>
-    <row r="10" spans="1:12" ht="28.5">
+    <row r="10" spans="1:12" ht="30">
       <c r="A10" s="15" t="s">
         <v>34</v>
       </c>
@@ -2167,13 +2167,13 @@
       <selection activeCell="E2" sqref="A2:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="35.73046875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.59765625" customWidth="1"/>
-    <col min="3" max="3" width="53.1328125" customWidth="1"/>
-    <col min="4" max="4" width="20.73046875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.5703125" customWidth="1"/>
+    <col min="3" max="3" width="53.140625" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:5">
@@ -2743,16 +2743,16 @@
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="48.73046875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.86328125" customWidth="1"/>
-    <col min="3" max="3" width="63.3984375" customWidth="1"/>
-    <col min="4" max="4" width="19.59765625" customWidth="1"/>
-    <col min="5" max="5" width="23.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="48.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.85546875" customWidth="1"/>
+    <col min="3" max="3" width="63.42578125" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" customWidth="1"/>
+    <col min="5" max="5" width="23.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" ht="17.649999999999999">
+    <row r="2" spans="1:5" ht="18">
       <c r="A2" s="40" t="s">
         <v>105</v>
       </c>
@@ -2869,13 +2869,13 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="40.265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" ht="18">
+    <row r="2" spans="1:2" ht="18.75">
       <c r="A2" s="1" t="s">
         <v>106</v>
       </c>
@@ -2899,7 +2899,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>